<commit_message>
add function to split xml files
</commit_message>
<xml_diff>
--- a/product/output/data_xml_to_excel.xlsx
+++ b/product/output/data_xml_to_excel.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CG3"/>
+  <dimension ref="A1:CG2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1275,433 +1275,6 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>official</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Thai</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Minh</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Khue</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>nickname</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Horse</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>phone</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>+84914002126</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>mobile</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>2000-12-04</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>home</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>34 Ngo Thoi Nham, Thuan Hoa, Hue, Thua Thien Hue 49000</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>34 Ngo Thoi Nham</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>Thuan Hoa</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>Hue</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>Thua Thien Hue</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>49000</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>2005</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>temporary</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>Samsora Riverside, Binh Thang, Di An, Binh Duong 75001</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>Samsora Riverside</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>Binh Thang</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>Di An</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>Binh Duong</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>75000</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>temporary</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>495/18/12 To Hien Thanh, 14, 10, Ho Chi Minh City 70001</t>
-        </is>
-      </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>495/18/12 To Hien Thanh</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="AH3" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="AI3" t="inlineStr">
-        <is>
-          <t>Ho Chi Minh City</t>
-        </is>
-      </c>
-      <c r="AJ3" t="inlineStr">
-        <is>
-          <t>70000</t>
-        </is>
-      </c>
-      <c r="AK3" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-      <c r="AL3" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
-      </c>
-      <c r="AM3" t="inlineStr">
-        <is>
-          <t>mom</t>
-        </is>
-      </c>
-      <c r="AN3" t="inlineStr">
-        <is>
-          <t>official</t>
-        </is>
-      </c>
-      <c r="AO3" t="inlineStr">
-        <is>
-          <t>Bui</t>
-        </is>
-      </c>
-      <c r="AP3" t="inlineStr">
-        <is>
-          <t>The</t>
-        </is>
-      </c>
-      <c r="AQ3" t="inlineStr">
-        <is>
-          <t>Ngoc Diep</t>
-        </is>
-      </c>
-      <c r="AR3" t="inlineStr">
-        <is>
-          <t>phone</t>
-        </is>
-      </c>
-      <c r="AS3" t="inlineStr">
-        <is>
-          <t>+84942440815</t>
-        </is>
-      </c>
-      <c r="AT3" t="inlineStr">
-        <is>
-          <t>mobile</t>
-        </is>
-      </c>
-      <c r="AU3" t="inlineStr">
-        <is>
-          <t>home</t>
-        </is>
-      </c>
-      <c r="AV3" t="inlineStr">
-        <is>
-          <t>34 Ngo Thoi Nham, Thuan Hoa, Hue, Thua Thien Hue 49000</t>
-        </is>
-      </c>
-      <c r="AW3" t="inlineStr">
-        <is>
-          <t>34 Ngo Thoi Nham</t>
-        </is>
-      </c>
-      <c r="AX3" t="inlineStr">
-        <is>
-          <t>Thuan Hoa</t>
-        </is>
-      </c>
-      <c r="AY3" t="inlineStr">
-        <is>
-          <t>Hue</t>
-        </is>
-      </c>
-      <c r="AZ3" t="inlineStr">
-        <is>
-          <t>Thua Thien Hue</t>
-        </is>
-      </c>
-      <c r="BA3" t="inlineStr">
-        <is>
-          <t>49000</t>
-        </is>
-      </c>
-      <c r="BB3" t="inlineStr">
-        <is>
-          <t>1999</t>
-        </is>
-      </c>
-      <c r="BC3" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
-      </c>
-      <c r="BD3" t="inlineStr">
-        <is>
-          <t>LK123123</t>
-        </is>
-      </c>
-      <c r="BE3" t="inlineStr">
-        <is>
-          <t>BN123124</t>
-        </is>
-      </c>
-      <c r="BF3" t="inlineStr">
-        <is>
-          <t>HS123124</t>
-        </is>
-      </c>
-      <c r="BG3" t="inlineStr">
-        <is>
-          <t>2020-12-04</t>
-        </is>
-      </c>
-      <c r="BH3" t="inlineStr">
-        <is>
-          <t>2021-12-04</t>
-        </is>
-      </c>
-      <c r="BI3" t="inlineStr">
-        <is>
-          <t>DKBD1001</t>
-        </is>
-      </c>
-      <c r="BJ3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="BK3" t="inlineStr">
-        <is>
-          <t>Kham Benh</t>
-        </is>
-      </c>
-      <c r="BL3" t="inlineStr">
-        <is>
-          <t>KHOA124</t>
-        </is>
-      </c>
-      <c r="BM3" t="inlineStr">
-        <is>
-          <t>CSKCB4</t>
-        </is>
-      </c>
-      <c r="BN3" t="inlineStr">
-        <is>
-          <t>K2</t>
-        </is>
-      </c>
-      <c r="BO3" t="inlineStr">
-        <is>
-          <t>PTTT124</t>
-        </is>
-      </c>
-      <c r="BP3" t="inlineStr">
-        <is>
-          <t>Covid-20</t>
-        </is>
-      </c>
-      <c r="BQ3" t="inlineStr">
-        <is>
-          <t>BENH2223</t>
-        </is>
-      </c>
-      <c r="BR3" t="inlineStr">
-        <is>
-          <t>BENHKHAC3334</t>
-        </is>
-      </c>
-      <c r="BS3" t="inlineStr">
-        <is>
-          <t>Dung Tuyen</t>
-        </is>
-      </c>
-      <c r="BT3" t="inlineStr">
-        <is>
-          <t>2019-08-04</t>
-        </is>
-      </c>
-      <c r="BU3" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
-      </c>
-      <c r="BV3" t="inlineStr">
-        <is>
-          <t>Chua khoi</t>
-        </is>
-      </c>
-      <c r="BW3" t="inlineStr">
-        <is>
-          <t>Ra vien</t>
-        </is>
-      </c>
-      <c r="BX3" t="inlineStr">
-        <is>
-          <t>2019-09-04</t>
-        </is>
-      </c>
-      <c r="BY3" t="inlineStr">
-        <is>
-          <t>12.34</t>
-        </is>
-      </c>
-      <c r="BZ3" t="inlineStr">
-        <is>
-          <t>13.24</t>
-        </is>
-      </c>
-      <c r="CA3" t="inlineStr">
-        <is>
-          <t>32.14</t>
-        </is>
-      </c>
-      <c r="CB3" t="inlineStr">
-        <is>
-          <t>23.14</t>
-        </is>
-      </c>
-      <c r="CC3" t="inlineStr">
-        <is>
-          <t>14.23</t>
-        </is>
-      </c>
-      <c r="CD3" t="inlineStr">
-        <is>
-          <t>42.13</t>
-        </is>
-      </c>
-      <c r="CE3" t="inlineStr">
-        <is>
-          <t>42.31</t>
-        </is>
-      </c>
-      <c r="CF3" t="inlineStr">
-        <is>
-          <t>43.12</t>
-        </is>
-      </c>
-      <c r="CG3" t="inlineStr">
-        <is>
-          <t>2019-09-02</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>